<commit_message>
Use US data for fuels/PEIIR
</commit_message>
<xml_diff>
--- a/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
+++ b/InputData/fuels/PEIIR/Pollutant Emissions Intensity Improvement Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\fuels\PEIIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\fuels\PEIIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C5BDB8-164C-4260-8BDD-310BFE54C72D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCB0351-311A-4D66-9EBD-A496CBB553FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21045" yWindow="1410" windowWidth="33360" windowHeight="21225" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="783" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>The U.S. EPS does not assume any improvement in pollutant emissions intensities over time,</t>
   </si>
   <si>
-    <t>so all rates are set to zero.</t>
-  </si>
-  <si>
     <t>kerosene</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Improvement Rate (dimensionless)</t>
+  </si>
+  <si>
+    <t>so all rates are set to zero. The EU model will carry the same assumption.</t>
   </si>
 </sst>
 </file>
@@ -701,35 +701,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,99 +739,99 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="A25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -847,22 +849,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.40625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.1328125" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
@@ -883,19 +885,19 @@
         <v>23</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -930,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -965,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1000,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1105,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1140,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1280,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1330,23 +1332,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A1" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>21</v>
@@ -1370,16 +1372,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1414,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1659,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1694,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1729,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1764,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1814,23 +1816,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -1854,16 +1856,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2038,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2073,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2108,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2143,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2178,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2298,23 +2300,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -2338,16 +2340,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2382,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2417,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2452,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2487,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2522,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2557,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2592,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2627,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2662,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2697,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2732,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2782,23 +2784,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -2822,16 +2824,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2936,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2971,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3041,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3076,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3111,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3146,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3181,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3216,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3266,23 +3268,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -3306,16 +3308,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3350,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3385,7 +3387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3420,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3490,7 +3492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3525,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3595,7 +3597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3630,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3665,7 +3667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3700,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3750,23 +3752,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.40625" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.1328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -3790,16 +3792,16 @@
         <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3834,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3869,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3904,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3939,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3974,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4009,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4079,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4114,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4149,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4184,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4234,27 +4236,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" customWidth="1"/>
+    <col min="11" max="11" width="16.1328125" customWidth="1"/>
+    <col min="12" max="12" width="20.7265625" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1328125" customWidth="1"/>
+    <col min="16" max="16" width="17.1328125" customWidth="1"/>
+    <col min="17" max="17" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>32</v>
@@ -4296,16 +4298,16 @@
         <v>35</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4358,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4411,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4517,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4570,7 +4572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4623,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4676,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4729,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4782,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4835,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4888,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4956,22 +4958,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="24.7265625" customWidth="1"/>
+    <col min="10" max="10" width="22.86328125" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -4992,19 +4994,19 @@
         <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5039,7 +5041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5109,7 +5111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5179,7 +5181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -5214,7 +5216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5284,7 +5286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5319,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5354,7 +5356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5389,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>

</xml_diff>